<commit_message>
finish with single form
</commit_message>
<xml_diff>
--- a/data/sample_data.xlsx
+++ b/data/sample_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Self\excel-to-word-filler\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C901AC0D-C95C-4BA6-B7A8-0CB79AAC6652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F703A92-5487-4A72-98A1-F17FC278DD5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{3EF6F02E-241D-4DBF-A7F7-1A067FB7F9E7}"/>
+    <workbookView xWindow="384" yWindow="384" windowWidth="17280" windowHeight="9960" xr2:uid="{3EF6F02E-241D-4DBF-A7F7-1A067FB7F9E7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>STT</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Số điện thoại</t>
   </si>
   <si>
-    <t>Nguyen Van A</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nguyen Van B </t>
   </si>
   <si>
@@ -78,6 +75,15 @@
   </si>
   <si>
     <t xml:space="preserve">nhà </t>
+  </si>
+  <si>
+    <t>Lê Thị Yến</t>
+  </si>
+  <si>
+    <t>Bắc Ninh</t>
+  </si>
+  <si>
+    <t>Hà Nội</t>
   </si>
 </sst>
 </file>
@@ -452,7 +458,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -476,7 +482,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -484,16 +490,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
       </c>
       <c r="D2">
         <v>444</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -501,7 +507,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>12</v>
@@ -510,7 +516,7 @@
         <v>555</v>
       </c>
       <c r="E3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -518,7 +524,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>12</v>
@@ -527,7 +533,7 @@
         <v>666</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -535,7 +541,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>12</v>
@@ -544,7 +550,7 @@
         <v>333</v>
       </c>
       <c r="E5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -552,7 +558,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>12</v>
@@ -561,7 +567,7 @@
         <v>343</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -569,7 +575,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7">
         <v>12</v>
@@ -578,7 +584,7 @@
         <v>335</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -586,7 +592,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8">
         <v>12</v>
@@ -595,7 +601,7 @@
         <v>3332</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>